<commit_message>
7th commit - on branch 1.0 - Updating "Dossier de conception fonctionnelle"
</commit_message>
<xml_diff>
--- a/resume_cas_utilisations.xlsx
+++ b/resume_cas_utilisations.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STEPHEN_AO\05_THE_PYTHON_APPLICATION_DEVELOPER\PROJECTS\04_Analyser_les_besoins_de_votre_client_pour_son_groupe_de_pizzerias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STEPHEN_AO\05_THE_PYTHON_APPLICATION_DEVELOPER\PROJECTS\04_Analyser_les_besoins_de_votre_client_pour_son_groupe_de_pizzerias\P4_Analysez_les_besoins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72789193-ED3E-4C26-A1CB-990FFF04BD90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE33BD1C-6EAB-485C-ACFB-E5071E194C75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cas d'utilisations" sheetId="1" r:id="rId1"/>
     <sheet name="Acteurs, Packages et CUs" sheetId="4" r:id="rId2"/>
-    <sheet name="Liste fonctionnalités" sheetId="5" r:id="rId3"/>
+    <sheet name="Les CU détaillées" sheetId="5" r:id="rId3"/>
+    <sheet name="Les CU généraux" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="94">
   <si>
     <t>INDICE</t>
   </si>
@@ -250,9 +251,6 @@
     <t>B3</t>
   </si>
   <si>
-    <t>B4</t>
-  </si>
-  <si>
     <t>B5</t>
   </si>
   <si>
@@ -289,9 +287,6 @@
     <t>Obtenir récapitulatif</t>
   </si>
   <si>
-    <t>Sélectionner une pizza disponible</t>
-  </si>
-  <si>
     <t>Payer à la livraison</t>
   </si>
   <si>
@@ -305,6 +300,24 @@
   </si>
   <si>
     <t>Back-Office</t>
+  </si>
+  <si>
+    <t>Gestion de commandes</t>
+  </si>
+  <si>
+    <t>Inspection de commandes</t>
+  </si>
+  <si>
+    <t>Gestion de matières premières</t>
+  </si>
+  <si>
+    <t>Inspection de matières premières</t>
+  </si>
+  <si>
+    <t>Consommateur</t>
+  </si>
+  <si>
+    <t>Enregitrement de commande</t>
   </si>
 </sst>
 </file>
@@ -388,12 +401,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -428,8 +435,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -741,19 +754,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -902,6 +902,132 @@
       </left>
       <right/>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashDot">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -911,7 +1037,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -957,207 +1083,261 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1261,7 +1441,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>701041</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1623,10 +1803,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="19">
+      <c r="A2" s="40">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1636,8 +1816,8 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1650,8 +1830,8 @@
       <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1663,8 +1843,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1693,10 +1873,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="17">
+      <c r="A7" s="41">
         <v>3</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="43" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1710,8 +1890,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1723,10 +1903,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
+      <c r="A9" s="41">
         <v>4</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="43" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1736,8 +1916,8 @@
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1745,8 +1925,8 @@
       <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1754,8 +1934,8 @@
       <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1763,10 +1943,10 @@
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
+      <c r="A13" s="41">
         <v>5</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1780,8 +1960,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1789,10 +1969,10 @@
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
+      <c r="A15" s="41">
         <v>6</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="43" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1806,8 +1986,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1819,8 +1999,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="43"/>
       <c r="C17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1850,16 +2030,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1870,7 +2050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71415E73-AB34-4D6B-8F8C-5A5045AA7DF9}">
   <dimension ref="B1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1898,94 +2078,94 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="21">
+      <c r="B3" s="17">
         <v>1</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="80" t="s">
+      <c r="E3" s="50" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21">
+      <c r="B4" s="17">
         <v>2</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="78"/>
-      <c r="E4" s="81"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="51"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="21">
+      <c r="B5" s="17">
         <v>3</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="78"/>
-      <c r="E5" s="81"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="51"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="21">
+      <c r="B6" s="17">
         <v>4</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="78"/>
-      <c r="E6" s="81"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="51"/>
     </row>
     <row r="7" spans="2:5" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="21">
+      <c r="B7" s="17">
         <v>5</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="79"/>
-      <c r="E7" s="82"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="52"/>
     </row>
     <row r="8" spans="2:5" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="21">
+      <c r="B8" s="17">
         <v>6</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="83" t="s">
+      <c r="E8" s="39" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="21">
+      <c r="B9" s="17">
         <v>7</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="75"/>
-      <c r="E9" s="83" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="21">
+      <c r="B10" s="17">
         <v>8</v>
       </c>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="76"/>
-      <c r="E10" s="83" t="s">
+      <c r="D10" s="49"/>
+      <c r="E10" s="39" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2002,10 +2182,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D377A1-F8B2-429F-813D-CFA4B93D7356}">
-  <dimension ref="B5:L36"/>
+  <dimension ref="B5:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2017,547 +2197,529 @@
   <sheetData>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="E6" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="K6" s="66"/>
-      <c r="L6" s="67"/>
+      <c r="E6" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" s="57"/>
+      <c r="L6" s="58"/>
     </row>
     <row r="7" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="26"/>
+      <c r="E7" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="66"/>
     </row>
     <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="70" t="s">
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="70" t="s">
+      <c r="F8" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="70" t="s">
+      <c r="G8" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="71" t="s">
+      <c r="I8" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="68" t="s">
+      <c r="J8" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="69" t="s">
+      <c r="K8" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="69" t="s">
+      <c r="L8" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="48"/>
-      <c r="C9" s="27" t="s">
+      <c r="B9" s="59"/>
+      <c r="C9" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="32"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="78"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="49"/>
-      <c r="C10" s="33" t="s">
+      <c r="B10" s="60"/>
+      <c r="C10" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="38"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="81"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="49"/>
-      <c r="C11" s="33" t="s">
+      <c r="B11" s="60"/>
+      <c r="C11" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="38"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="81"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="49"/>
-      <c r="C12" s="33" t="s">
+      <c r="B12" s="60"/>
+      <c r="C12" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="38"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="81"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="49"/>
-      <c r="C13" s="33" t="s">
+      <c r="B13" s="60"/>
+      <c r="C13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="38"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="81"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="49"/>
-      <c r="C14" s="33" t="s">
+      <c r="B14" s="60"/>
+      <c r="C14" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="38"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="81"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="49"/>
-      <c r="C15" s="33" t="s">
+      <c r="B15" s="60"/>
+      <c r="C15" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="85"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="81"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="60"/>
+      <c r="C16" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="38"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="49"/>
-      <c r="C16" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="34" t="s">
+      <c r="E16" s="85"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="81"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="60"/>
+      <c r="C17" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="85"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="84"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="80"/>
+      <c r="L17" s="81"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="60"/>
+      <c r="C18" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="38"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="49"/>
-      <c r="C17" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="38"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="49"/>
-      <c r="C18" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="34" t="s">
+      <c r="E18" s="85"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="80"/>
+      <c r="L18" s="81"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="60"/>
+      <c r="C19" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="93" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="85"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="81"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="60"/>
+      <c r="C20" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="93" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="38"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="49"/>
-      <c r="C19" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="38"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="49"/>
-      <c r="C20" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="34" t="s">
+      <c r="E20" s="85"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="84"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="81"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="60"/>
+      <c r="C21" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="93" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="85"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="84"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="81"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="60"/>
+      <c r="C22" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="85"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="81"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="60"/>
+      <c r="C23" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="85"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="60"/>
+      <c r="C24" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="93" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="85"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="84"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="80"/>
+      <c r="L24" s="24"/>
+    </row>
+    <row r="25" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="61"/>
+      <c r="C25" s="94" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="95" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="96"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="97"/>
+      <c r="I25" s="98"/>
+      <c r="J25" s="99"/>
+      <c r="K25" s="97"/>
+      <c r="L25" s="100"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="101"/>
+      <c r="C26" s="90" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="78"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="102"/>
+      <c r="C27" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="38"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="49"/>
-      <c r="C21" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="38"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="49"/>
-      <c r="C22" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="38"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="49"/>
-      <c r="C23" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="40"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="49"/>
-      <c r="C24" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="40"/>
-    </row>
-    <row r="25" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="50"/>
-      <c r="C25" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="40"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="51"/>
-      <c r="C26" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="38"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="52"/>
-      <c r="C27" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="42" t="s">
+      <c r="E27" s="22"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="84"/>
+      <c r="J27" s="79"/>
+      <c r="K27" s="80"/>
+      <c r="L27" s="81"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="102"/>
+      <c r="C28" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="38"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="52"/>
-      <c r="C28" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="42" t="s">
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="79"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="81"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="102"/>
+      <c r="C29" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="22"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="81"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="102"/>
+      <c r="C30" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="22"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="80"/>
+      <c r="I30" s="84"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="80"/>
+      <c r="L30" s="81"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" s="102"/>
+      <c r="C31" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="22"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="79"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="81"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B32" s="102"/>
+      <c r="C32" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="61"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="38"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="52"/>
-      <c r="C29" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="38"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="52"/>
-      <c r="C30" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="42" t="s">
+      <c r="E32" s="22"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="84"/>
+      <c r="J32" s="79"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="81"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B33" s="102"/>
+      <c r="C33" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="85"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="84"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="24"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B34" s="102"/>
+      <c r="C34" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="85"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="24"/>
+    </row>
+    <row r="35" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="103"/>
+      <c r="C35" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="38"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="52"/>
-      <c r="C31" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="37"/>
-      <c r="L31" s="38"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="52"/>
-      <c r="C32" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="35"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="57"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="38"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="52"/>
-      <c r="C33" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="35"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="38"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="52"/>
-      <c r="C34" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="40"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B35" s="52"/>
-      <c r="C35" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="D35" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="40"/>
-    </row>
-    <row r="36" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="53"/>
-      <c r="C36" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="45"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="63"/>
-      <c r="J36" s="59"/>
-      <c r="K36" s="46"/>
-      <c r="L36" s="47"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="87"/>
+      <c r="G35" s="87"/>
+      <c r="H35" s="87"/>
+      <c r="I35" s="87"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="87"/>
+      <c r="L35" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="E6:I6"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="B9:B25"/>
-    <mergeCell ref="B26:B36"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:L7"/>
@@ -2565,4 +2727,183 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148406FD-A831-4BBC-B3E8-1A0BB125CE3D}">
+  <dimension ref="B5:J16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:10" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C6" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="57"/>
+      <c r="J6" s="58"/>
+    </row>
+    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="66"/>
+    </row>
+    <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="63"/>
+      <c r="C8" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="78"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="81"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="81"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="81"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="85"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="24"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="85"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="84"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="24"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="85"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="24"/>
+    </row>
+    <row r="16" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="82"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:J7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
9th commit - on branch 1.0 - Finishing "Dossier de conception fonctionnelle" 1.0. - Finishing README.md 1.0
</commit_message>
<xml_diff>
--- a/resume_cas_utilisations.xlsx
+++ b/resume_cas_utilisations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STEPHEN_AO\05_THE_PYTHON_APPLICATION_DEVELOPER\PROJECTS\04_Analyser_les_besoins_de_votre_client_pour_son_groupe_de_pizzerias\P4_Analysez_les_besoins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE33BD1C-6EAB-485C-ACFB-E5071E194C75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5004101-F52E-40DD-B370-16AAB51E2EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Cas d'utilisations" sheetId="1" r:id="rId1"/>
     <sheet name="Acteurs, Packages et CUs" sheetId="4" r:id="rId2"/>
     <sheet name="Les CU détaillées" sheetId="5" r:id="rId3"/>
-    <sheet name="Les CU généraux" sheetId="7" r:id="rId4"/>
+    <sheet name="Feuil1" sheetId="8" r:id="rId4"/>
+    <sheet name="Les CU généraux" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -442,7 +443,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -934,19 +935,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="mediumDashDot">
         <color indexed="64"/>
       </left>
@@ -1037,7 +1025,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1152,111 +1140,15 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1299,13 +1191,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1320,6 +1212,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1329,15 +1224,102 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1803,10 +1785,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="40">
+      <c r="A2" s="74">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="75" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1816,8 +1798,8 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="41"/>
-      <c r="B3" s="43"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="73"/>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1830,8 +1812,8 @@
       <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="41"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="72"/>
+      <c r="B4" s="73"/>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1843,8 +1825,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
-      <c r="B5" s="43"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1873,10 +1855,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="41">
+      <c r="A7" s="72">
         <v>3</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="73" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1890,8 +1872,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="41"/>
-      <c r="B8" s="43"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1903,10 +1885,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="41">
+      <c r="A9" s="72">
         <v>4</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="73" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1916,8 +1898,8 @@
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
-      <c r="B10" s="43"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1925,8 +1907,8 @@
       <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="41"/>
-      <c r="B11" s="43"/>
+      <c r="A11" s="72"/>
+      <c r="B11" s="73"/>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1934,8 +1916,8 @@
       <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1943,10 +1925,10 @@
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="41">
+      <c r="A13" s="72">
         <v>5</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="73" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1960,8 +1942,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="41"/>
-      <c r="B14" s="43"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="73"/>
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1969,10 +1951,10 @@
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="41">
+      <c r="A15" s="72">
         <v>6</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="73" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1986,8 +1968,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
-      <c r="B16" s="43"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1999,8 +1981,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="41"/>
-      <c r="B17" s="43"/>
+      <c r="A17" s="72"/>
+      <c r="B17" s="73"/>
       <c r="C17" s="1" t="s">
         <v>23</v>
       </c>
@@ -2084,10 +2066,10 @@
       <c r="C3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="82" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2098,8 +2080,8 @@
       <c r="C4" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="51"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="83"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="17">
@@ -2108,8 +2090,8 @@
       <c r="C5" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="51"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="83"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="17">
@@ -2118,8 +2100,8 @@
       <c r="C6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="51"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="83"/>
     </row>
     <row r="7" spans="2:5" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17">
@@ -2128,8 +2110,8 @@
       <c r="C7" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="52"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="84"/>
     </row>
     <row r="8" spans="2:5" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="17">
@@ -2138,7 +2120,7 @@
       <c r="C8" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="79" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="39" t="s">
@@ -2152,7 +2134,7 @@
       <c r="C9" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="48"/>
+      <c r="D9" s="80"/>
       <c r="E9" s="39" t="s">
         <v>47</v>
       </c>
@@ -2164,7 +2146,7 @@
       <c r="C10" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="49"/>
+      <c r="D10" s="81"/>
       <c r="E10" s="39" t="s">
         <v>49</v>
       </c>
@@ -2185,52 +2167,56 @@
   <dimension ref="B5:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+      <selection activeCell="P29" sqref="P28:P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="56" t="s">
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88" t="s">
         <v>87</v>
       </c>
-      <c r="K6" s="57"/>
-      <c r="L6" s="58"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="90"/>
     </row>
     <row r="7" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="96" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="66"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="98"/>
     </row>
     <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
       <c r="E8" s="35" t="s">
         <v>3</v>
       </c>
@@ -2246,7 +2232,7 @@
       <c r="I8" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="89" t="s">
+      <c r="J8" s="57" t="s">
         <v>6</v>
       </c>
       <c r="K8" s="34" t="s">
@@ -2257,313 +2243,313 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="59"/>
+      <c r="B9" s="91"/>
       <c r="C9" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="92" t="s">
+      <c r="D9" s="60" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="78"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="46"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="60"/>
+      <c r="B10" s="92"/>
       <c r="C10" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="93" t="s">
+      <c r="D10" s="61" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="81"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="49"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="60"/>
+      <c r="B11" s="92"/>
       <c r="C11" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="93" t="s">
+      <c r="D11" s="61" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="81"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="49"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="60"/>
+      <c r="B12" s="92"/>
       <c r="C12" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="93" t="s">
+      <c r="D12" s="61" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="81"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="49"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="60"/>
+      <c r="B13" s="92"/>
       <c r="C13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="93" t="s">
+      <c r="D13" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="85"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
       <c r="H13" s="23"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="81"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="49"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="60"/>
+      <c r="B14" s="92"/>
       <c r="C14" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="93" t="s">
+      <c r="D14" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="85"/>
-      <c r="F14" s="80"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="48"/>
       <c r="G14" s="23"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="79"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="81"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="49"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="60"/>
+      <c r="B15" s="92"/>
       <c r="C15" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="93" t="s">
+      <c r="D15" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="85"/>
-      <c r="F15" s="80"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="48"/>
       <c r="G15" s="23"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="81"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="49"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="60"/>
+      <c r="B16" s="92"/>
       <c r="C16" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="93" t="s">
+      <c r="D16" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="85"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="84"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="52"/>
       <c r="J16" s="30"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="81"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="49"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="60"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="93" t="s">
+      <c r="D17" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="85"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="84"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="52"/>
       <c r="J17" s="30"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="81"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="49"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="60"/>
+      <c r="B18" s="92"/>
       <c r="C18" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="93" t="s">
+      <c r="D18" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="85"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="80"/>
-      <c r="I18" s="84"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="52"/>
       <c r="J18" s="30"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="81"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="49"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="60"/>
+      <c r="B19" s="92"/>
       <c r="C19" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="93" t="s">
+      <c r="D19" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="85"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="80"/>
-      <c r="I19" s="84"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="52"/>
       <c r="J19" s="30"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="81"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="49"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="60"/>
+      <c r="B20" s="92"/>
       <c r="C20" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="93" t="s">
+      <c r="D20" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="85"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="84"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="52"/>
       <c r="J20" s="30"/>
-      <c r="K20" s="80"/>
-      <c r="L20" s="81"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="49"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="60"/>
+      <c r="B21" s="92"/>
       <c r="C21" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="93" t="s">
+      <c r="D21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="85"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="80"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="79"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="47"/>
       <c r="K21" s="23"/>
-      <c r="L21" s="81"/>
+      <c r="L21" s="49"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="60"/>
+      <c r="B22" s="92"/>
       <c r="C22" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="93" t="s">
+      <c r="D22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="85"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="79"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="47"/>
       <c r="K22" s="23"/>
-      <c r="L22" s="81"/>
+      <c r="L22" s="49"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="60"/>
+      <c r="B23" s="92"/>
       <c r="C23" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="93" t="s">
+      <c r="D23" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="85"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="80"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="80"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="48"/>
       <c r="L23" s="24"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="60"/>
+      <c r="B24" s="92"/>
       <c r="C24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="93" t="s">
+      <c r="D24" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="85"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="80"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="48"/>
       <c r="L24" s="24"/>
     </row>
     <row r="25" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="61"/>
-      <c r="C25" s="94" t="s">
+      <c r="B25" s="93"/>
+      <c r="C25" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="95" t="s">
+      <c r="D25" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="96"/>
-      <c r="F25" s="97"/>
-      <c r="G25" s="97"/>
-      <c r="H25" s="97"/>
-      <c r="I25" s="98"/>
-      <c r="J25" s="99"/>
-      <c r="K25" s="97"/>
-      <c r="L25" s="100"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="68"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="101"/>
-      <c r="C26" s="90" t="s">
+      <c r="B26" s="69"/>
+      <c r="C26" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="91" t="s">
+      <c r="D26" s="59" t="s">
         <v>26</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="76"/>
-      <c r="K26" s="77"/>
-      <c r="L26" s="78"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="46"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="102"/>
+      <c r="B27" s="70"/>
       <c r="C27" s="25" t="s">
         <v>68</v>
       </c>
@@ -2573,14 +2559,14 @@
       <c r="E27" s="22"/>
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="79"/>
-      <c r="K27" s="80"/>
-      <c r="L27" s="81"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="49"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="102"/>
+      <c r="B28" s="70"/>
       <c r="C28" s="25" t="s">
         <v>69</v>
       </c>
@@ -2590,14 +2576,14 @@
       <c r="E28" s="22"/>
       <c r="F28" s="23"/>
       <c r="G28" s="23"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="80"/>
-      <c r="L28" s="81"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="49"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="102"/>
+      <c r="B29" s="70"/>
       <c r="C29" s="25" t="s">
         <v>70</v>
       </c>
@@ -2607,14 +2593,14 @@
       <c r="E29" s="22"/>
       <c r="F29" s="23"/>
       <c r="G29" s="23"/>
-      <c r="H29" s="80"/>
-      <c r="I29" s="84"/>
-      <c r="J29" s="79"/>
-      <c r="K29" s="80"/>
-      <c r="L29" s="81"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="49"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="102"/>
+      <c r="B30" s="70"/>
       <c r="C30" s="25" t="s">
         <v>71</v>
       </c>
@@ -2624,14 +2610,14 @@
       <c r="E30" s="22"/>
       <c r="F30" s="23"/>
       <c r="G30" s="23"/>
-      <c r="H30" s="80"/>
-      <c r="I30" s="84"/>
-      <c r="J30" s="79"/>
-      <c r="K30" s="80"/>
-      <c r="L30" s="81"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="49"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="102"/>
+      <c r="B31" s="70"/>
       <c r="C31" s="25" t="s">
         <v>72</v>
       </c>
@@ -2639,16 +2625,16 @@
         <v>27</v>
       </c>
       <c r="E31" s="22"/>
-      <c r="F31" s="80"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="23"/>
-      <c r="H31" s="80"/>
+      <c r="H31" s="48"/>
       <c r="I31" s="32"/>
-      <c r="J31" s="79"/>
-      <c r="K31" s="80"/>
-      <c r="L31" s="81"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="49"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="102"/>
+      <c r="B32" s="70"/>
       <c r="C32" s="25" t="s">
         <v>73</v>
       </c>
@@ -2656,63 +2642,63 @@
         <v>83</v>
       </c>
       <c r="E32" s="22"/>
-      <c r="F32" s="80"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="23"/>
-      <c r="H32" s="80"/>
-      <c r="I32" s="84"/>
-      <c r="J32" s="79"/>
-      <c r="K32" s="80"/>
-      <c r="L32" s="81"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="49"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="102"/>
+      <c r="B33" s="70"/>
       <c r="C33" s="25" t="s">
         <v>74</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="85"/>
+      <c r="E33" s="53"/>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>
-      <c r="H33" s="80"/>
-      <c r="I33" s="84"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="52"/>
       <c r="J33" s="30"/>
       <c r="K33" s="23"/>
       <c r="L33" s="24"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="102"/>
+      <c r="B34" s="70"/>
       <c r="C34" s="25" t="s">
         <v>75</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="85"/>
-      <c r="F34" s="80"/>
-      <c r="G34" s="80"/>
-      <c r="H34" s="80"/>
-      <c r="I34" s="80"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
       <c r="J34" s="30"/>
-      <c r="K34" s="80"/>
+      <c r="K34" s="48"/>
       <c r="L34" s="24"/>
     </row>
     <row r="35" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="103"/>
+      <c r="B35" s="71"/>
       <c r="C35" s="27" t="s">
         <v>76</v>
       </c>
       <c r="D35" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="86"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="87"/>
-      <c r="I35" s="87"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="55"/>
       <c r="J35" s="31"/>
-      <c r="K35" s="87"/>
+      <c r="K35" s="55"/>
       <c r="L35" s="29"/>
     </row>
   </sheetData>
@@ -2730,11 +2716,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B595B271-C2B0-40D4-A428-B5301EF7492A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148406FD-A831-4BBC-B3E8-1A0BB125CE3D}">
   <dimension ref="B5:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2745,43 +2743,43 @@
   <sheetData>
     <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:10" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56" t="s">
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="88" t="s">
         <v>87</v>
       </c>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="90"/>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="96" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="66"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="98"/>
     </row>
     <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="63"/>
-      <c r="C8" s="72" t="s">
+      <c r="B8" s="95"/>
+      <c r="C8" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="74"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="101"/>
       <c r="H8" s="33" t="s">
         <v>6</v>
       </c>
@@ -2793,20 +2791,20 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="78"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="46"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="41" t="s">
         <v>93</v>
       </c>
       <c r="C10" s="22"/>
@@ -2814,12 +2812,12 @@
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
       <c r="G10" s="32"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="81"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="49"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="41" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="22"/>
@@ -2827,12 +2825,12 @@
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
       <c r="G11" s="32"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="81"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="49"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="41" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="22"/>
@@ -2840,61 +2838,61 @@
       <c r="E12" s="23"/>
       <c r="F12" s="23"/>
       <c r="G12" s="32"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="81"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="49"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="85"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="80"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
       <c r="J13" s="24"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="85"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="84"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="52"/>
       <c r="H14" s="30"/>
-      <c r="I14" s="80"/>
+      <c r="I14" s="48"/>
       <c r="J14" s="24"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="85"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="84"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="52"/>
       <c r="H15" s="30"/>
-      <c r="I15" s="80"/>
+      <c r="I15" s="48"/>
       <c r="J15" s="24"/>
     </row>
     <row r="16" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="86"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="83"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="51"/>
       <c r="H16" s="31"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="82"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>